<commit_message>
CAN1-58 Updated microcontroller interface test cases by Antonio
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/Microcontroller_IF_Test_Cases.xlsx
+++ b/Documentations/Test Cases/Microcontroller_IF_Test_Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E1DE0A-C761-48B6-AA7A-3CFCB28AC86B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582244FB-D837-41EC-A1CF-D64C3441C0CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{158D7137-19E1-4EBC-9C77-2DF826506FBB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="320">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -994,10 +994,6 @@
 i_cs = 1
 i_r_neg_w = 1
 i_addr = 0x17</t>
-  </si>
-  <si>
-    <t>o_rs_vector at bit position 22 is set to 1 for one clock cycle if
-i_sys_clk transitions from 0 to 1 when i_cs and i_r_neg_w are 1 and i_addr is 0x618, else its set to 0</t>
   </si>
   <si>
     <t>o_rs_vector at bit position 23 is set to 1 for one clock cycle if
@@ -1702,6 +1698,802 @@
 4. Observe o_error is 0</t>
   </si>
   <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 0
+i_reg_ack = 0
+i_addr = 0x30
+i_reg_r_data = 0xAAAA_AAAA
+Second Check:
+i_cs = 1
+i_r_neg_w = 0
+i_reg_ack = 0
+i_addr = 0x30
+Third Check:
+i_cs = 0
+i_r_neg_w = 1
+i_reg_ack = 0
+i_addr = 0x30
+Fourth Check:
+i_cs = 0
+i_r_neg_w = 1
+i_reg_ack = 0
+i_addr = 0x00
+Fifth Check:
+i_cs = 0
+i_r_neg_w = 1
+i_reg_ack = 1
+i_addr = 0x00
+Sixth Check:
+i_cs = 1
+i_r_neg_w = 1
+i_reg_ack = 1
+i_addr = 0x00</t>
+  </si>
+  <si>
+    <t>First Check:
+o_reg_data = 0x0000_0000
+Second Check:
+o_reg_data = 0x0000_0000
+Third Check:
+o_reg_data = 0x0000_0000
+Fourht Check:
+o_reg_data = 0x0000_0000
+Fifth Check:
+o_reg_data = 0x0000_0000
+Sixth Check:
+o_reg_data = 0xAAAA_AAAA</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x30
+i_bus_data = 0xAAAA_AAAA
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x30
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x30
+Fourth Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fifth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x00</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x30
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x30
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x30
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x00</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x01</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x02</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0C</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x05</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x08</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x09</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0A</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0B</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0D</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0E</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x0F</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x10</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x11</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x18</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x19</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1A</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1B</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1C</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1D</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1E</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x1F</t>
+  </si>
+  <si>
+    <t>First Check:
+i_cs = 0
+i_r_neg_w = 1
+i_addr = 0x00
+Second Check:
+i_cs = 1
+i_r_neg_w = 1
+i_addr = 0x00
+Third Check:
+i_cs = 0
+i_r_neg_w = 0
+i_addr = 0x00
+Fourth Check:
+i_cs = 1
+i_r_neg_w = 0
+i_addr = 0x20</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x30
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x00
+11. Observe o_rs_vector at bit position 0 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
+10. Set i_cs to 0 and addr to 0x01
+11. Observe o_rs_vector at bit position 1 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x02
+11. Observe o_rs_vector at bit position 2 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x03
+11. Observe o_rs_vector at bit position 3 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x05
+11. Observe o_rs_vector at bit position 5 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x08
+11. Observe o_rs_vector at bit position 8 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x09
+11. Observe o_rs_vector at bit position 9 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0A
+11. Observe o_rs_vector at bit position 10 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0B
+11. Observe o_rs_vector at bit position 11 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0C
+11. Observe o_rs_vector at bit position 12 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0D
+11. Observe o_rs_vector at bit position 13 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0E
+11. Observe o_rs_vector at bit position 14 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x0F
+11. Observe o_rs_vector at bit position 15 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x10
+11. Observe o_rs_vector at bit position 16 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x11
+11. Observe o_rs_vector at bit position 17 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x18
+11. Observe o_rs_vector at bit position 22 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x19
+11. Observe o_rs_vector at bit position 23 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1A
+11. Observe o_rs_vector at bit position 24 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1B
+11. Observe o_rs_vector at bit position 25 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1C
+11. Observe o_rs_vector at bit position 26 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1D
+11. Observe o_rs_vector at bit position 27 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1E
+11. Observe o_rs_vector at bit position 28 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x1F
+11. Observe o_rs_vector at bit position 29 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
+    <t>1. Set i_reset to 1
+2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
+3. Wait for one clock cycle
+4. Set i_reset to 0
+5. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
+6. Set i_cs to 1
+7. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
+8. Set i_cs to 0 and i_r_neg_w to 0
+9. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
+10. Set i_cs to 1 and addr to 0x20
+11. Observe o_rs_vector at bit position 30 is set to 1 after one clock cycle</t>
+  </si>
+  <si>
     <t>1. Set i_reg_r_data to 0xAAAA_AAAA, i_cs to 0, i_reg_ack to 0, and i_r_neg_w to 0, and i_addr to 0x30
 2. Set i_reset to 0 after one clock cycle
 3. Wait for one clock cycle
@@ -1714,804 +2506,8 @@
 10. Observe that o_reg_data outputs 0x0000_0000 after one clock cycle
 11. Set i_reg_ack to 1
 12. Observe that o_reg_data outputs 0x0000_0000 after one clock cycle
-11. Set i_cs to 1
-12. Observe that o_reg_data outputs 0xAAAA_AAAA after one clock cycle.</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 0
-i_reg_ack = 0
-i_addr = 0x30
-i_reg_r_data = 0xAAAA_AAAA
-Second Check:
-i_cs = 1
-i_r_neg_w = 0
-i_reg_ack = 0
-i_addr = 0x30
-Third Check:
-i_cs = 0
-i_r_neg_w = 1
-i_reg_ack = 0
-i_addr = 0x30
-Fourth Check:
-i_cs = 0
-i_r_neg_w = 1
-i_reg_ack = 0
-i_addr = 0x00
-Fifth Check:
-i_cs = 0
-i_r_neg_w = 1
-i_reg_ack = 1
-i_addr = 0x00
-Sixth Check:
-i_cs = 1
-i_r_neg_w = 1
-i_reg_ack = 1
-i_addr = 0x00</t>
-  </si>
-  <si>
-    <t>First Check:
-o_reg_data = 0x0000_0000
-Second Check:
-o_reg_data = 0x0000_0000
-Third Check:
-o_reg_data = 0x0000_0000
-Fourht Check:
-o_reg_data = 0x0000_0000
-Fifth Check:
-o_reg_data = 0x0000_0000
-Sixth Check:
-o_reg_data = 0xAAAA_AAAA</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x30
-i_bus_data = 0xAAAA_AAAA
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x30
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x30
-Fourth Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fifth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x00</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x30
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x30
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x30
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x00</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x01</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x02</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0C</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x05</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x08</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x09</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0A</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0B</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0D</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0E</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x0F</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x10</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x11</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x18</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x19</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1A</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1B</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1C</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1D</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1E</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x1F</t>
-  </si>
-  <si>
-    <t>First Check:
-i_cs = 0
-i_r_neg_w = 1
-i_addr = 0x00
-Second Check:
-i_cs = 1
-i_r_neg_w = 1
-i_addr = 0x00
-Third Check:
-i_cs = 0
-i_r_neg_w = 0
-i_addr = 0x00
-Fourth Check:
-i_cs = 1
-i_r_neg_w = 0
-i_addr = 0x20</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x30
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 0 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x00
-11. Observe o_rs_vector at bit position 0 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 1 is set to 0 after one clock cycle
-10. Set i_cs to 0 and addr to 0x01
-11. Observe o_rs_vector at bit position 1 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 2 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x02
-11. Observe o_rs_vector at bit position 2 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 3 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x03
-11. Observe o_rs_vector at bit position 3 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 5 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x05
-11. Observe o_rs_vector at bit position 5 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 8 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x08
-11. Observe o_rs_vector at bit position 8 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 9 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x09
-11. Observe o_rs_vector at bit position 9 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 10 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0A
-11. Observe o_rs_vector at bit position 10 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 11 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0B
-11. Observe o_rs_vector at bit position 11 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 12 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0C
-11. Observe o_rs_vector at bit position 12 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 13 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0D
-11. Observe o_rs_vector at bit position 13 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 14 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0E
-11. Observe o_rs_vector at bit position 14 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 15 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x0F
-11. Observe o_rs_vector at bit position 15 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 16 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x10
-11. Observe o_rs_vector at bit position 16 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 17 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x11
-11. Observe o_rs_vector at bit position 17 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 22 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x18
-11. Observe o_rs_vector at bit position 22 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 23 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x19
-11. Observe o_rs_vector at bit position 23 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 24 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1A
-11. Observe o_rs_vector at bit position 24 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 25 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1B
-11. Observe o_rs_vector at bit position 25 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 26 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1C
-11. Observe o_rs_vector at bit position 26 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 27 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1D
-11. Observe o_rs_vector at bit position 27 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 28 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1E
-11. Observe o_rs_vector at bit position 28 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 29 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x1F
-11. Observe o_rs_vector at bit position 29 is set to 1 after one clock cycle</t>
-  </si>
-  <si>
-    <t>1. Set i_reset to 1
-2. Set i_cs to 0, i_r_neg_w to 1, and addr to 0x00
-3. Wait for one clock cycle
-4. Set i_reset to 0
-5. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
-6. Set i_cs to 1
-7. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
-8. Set i_cs to 0 and i_r_neg_w to 0
-9. Observe o_rs_vector at bit position 30 is set to 0 after one clock cycle
-10. Set i_cs to 1 and addr to 0x20
-11. Observe o_rs_vector at bit position 30 is set to 1 after one clock cycle</t>
+13. Set i_cs to 1
+14. Observe that o_reg_data outputs 0xAAAA_AAAA after one clock cycle.</t>
   </si>
 </sst>
 </file>
@@ -2883,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32681D7-96D8-42F8-A261-646649F540D1}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,13 +3056,13 @@
         <v>172</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3126,7 +3122,7 @@
         <v>174</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="285" x14ac:dyDescent="0.25">
@@ -3146,7 +3142,7 @@
         <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="285" x14ac:dyDescent="0.25">
@@ -3160,13 +3156,13 @@
         <v>178</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>179</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="285" x14ac:dyDescent="0.25">
@@ -3180,13 +3176,13 @@
         <v>180</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>181</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="285" x14ac:dyDescent="0.25">
@@ -3200,7 +3196,7 @@
         <v>182</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>155</v>
@@ -3220,7 +3216,7 @@
         <v>183</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>184</v>
@@ -3240,7 +3236,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>186</v>
@@ -3260,7 +3256,7 @@
         <v>187</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>188</v>
@@ -3280,7 +3276,7 @@
         <v>189</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>156</v>
@@ -3300,7 +3296,7 @@
         <v>190</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>162</v>
@@ -3320,7 +3316,7 @@
         <v>191</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>192</v>
@@ -3340,7 +3336,7 @@
         <v>193</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>194</v>
@@ -3360,7 +3356,7 @@
         <v>195</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>196</v>
@@ -3377,16 +3373,16 @@
         <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3397,16 +3393,16 @@
         <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3417,16 +3413,16 @@
         <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3437,16 +3433,16 @@
         <v>58</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3457,16 +3453,16 @@
         <v>60</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>164</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3477,16 +3473,16 @@
         <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3497,16 +3493,16 @@
         <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3517,16 +3513,16 @@
         <v>66</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3537,16 +3533,16 @@
         <v>68</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="375" x14ac:dyDescent="0.25">
@@ -3557,13 +3553,13 @@
         <v>70</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>170</v>
@@ -3620,13 +3616,13 @@
         <v>171</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3640,13 +3636,13 @@
         <v>175</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3660,13 +3656,13 @@
         <v>178</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3680,13 +3676,13 @@
         <v>180</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3700,10 +3696,10 @@
         <v>183</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>159</v>
@@ -3720,10 +3716,10 @@
         <v>189</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>165</v>
@@ -3737,16 +3733,16 @@
         <v>88</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3757,16 +3753,16 @@
         <v>90</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3777,16 +3773,16 @@
         <v>92</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3797,16 +3793,16 @@
         <v>94</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3817,16 +3813,16 @@
         <v>96</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3837,16 +3833,16 @@
         <v>98</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3857,16 +3853,16 @@
         <v>100</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3877,16 +3873,16 @@
         <v>102</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3897,16 +3893,16 @@
         <v>104</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3917,16 +3913,16 @@
         <v>106</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3937,16 +3933,16 @@
         <v>108</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3957,16 +3953,16 @@
         <v>110</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3977,16 +3973,16 @@
         <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -3997,16 +3993,16 @@
         <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -4017,16 +4013,16 @@
         <v>116</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -4037,16 +4033,16 @@
         <v>118</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -4057,16 +4053,16 @@
         <v>120</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="285" x14ac:dyDescent="0.25">
@@ -4077,16 +4073,16 @@
         <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -4097,16 +4093,16 @@
         <v>124</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>